<commit_message>
sorting order sort algorithm, 테이블 수정
</commit_message>
<xml_diff>
--- a/Project_C/Assets/ExcelTable/CardTable.xlsx
+++ b/Project_C/Assets/ExcelTable/CardTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOW2_400_204\Desktop\TeamIdentity\Project_C\Assets\ExcelTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Main\TeamIdentity\Project_C\Assets\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D2DEA7-1105-4305-BD16-88337D6BCB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="3"/>
+    <workbookView xWindow="4350" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnumTable" sheetId="4" r:id="rId1"/>
@@ -22,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="215">
   <si>
     <t>i_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -822,13 +815,57 @@
   </si>
   <si>
     <t>Sprites/Card/card_counter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardRangeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_PlayerRelativeCircularSector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_PointCircularSector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardRangeType_RangeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범위 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범위 파라미터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_RangeParameter[3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파라미터 x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파라미터 0 : angle, 1 : distance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_CardRangeSprite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범위 스프라이트 이미지 경로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -860,7 +897,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -894,13 +931,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -922,11 +968,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1308,17 +1426,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1671,6 +1790,48 @@
       </c>
       <c r="C32">
         <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" t="s">
+        <v>205</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1848,12 +2009,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:B20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B20">
     <sortCondition ref="B3:B20"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1863,7 +2024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2065,7 +2226,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2075,10 +2236,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2093,9 +2256,12 @@
     <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.75" customWidth="1"/>
     <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2131,8 +2297,19 @@
         <v>187</v>
       </c>
       <c r="M1" s="6"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2172,8 +2349,19 @@
       <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>301</v>
       </c>
@@ -2213,8 +2401,21 @@
       <c r="M3" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="12"/>
+      <c r="O3" t="s">
+        <v>205</v>
+      </c>
+      <c r="P3">
+        <v>160</v>
+      </c>
+      <c r="Q3">
+        <v>1.8</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>302</v>
       </c>
@@ -2254,8 +2455,15 @@
       <c r="M4" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" s="12"/>
+      <c r="O4" t="s">
+        <v>89</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>303</v>
       </c>
@@ -2295,8 +2503,15 @@
       <c r="M5" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" s="12"/>
+      <c r="O5" t="s">
+        <v>89</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>304</v>
       </c>
@@ -2336,8 +2551,15 @@
       <c r="M6" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" s="12"/>
+      <c r="O6" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>305</v>
       </c>
@@ -2377,8 +2599,15 @@
       <c r="M7" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" s="12"/>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>306</v>
       </c>
@@ -2418,8 +2647,15 @@
       <c r="M8" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" s="12"/>
+      <c r="O8" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>307</v>
       </c>
@@ -2459,8 +2695,15 @@
       <c r="M9" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" s="12"/>
+      <c r="O9" t="s">
+        <v>89</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>308</v>
       </c>
@@ -2500,8 +2743,15 @@
       <c r="M10" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10" s="12"/>
+      <c r="O10" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>309</v>
       </c>
@@ -2541,8 +2791,15 @@
       <c r="M11" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11" s="12"/>
+      <c r="O11" t="s">
+        <v>89</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>310</v>
       </c>
@@ -2582,8 +2839,21 @@
       <c r="M12" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" s="12"/>
+      <c r="O12" t="s">
+        <v>205</v>
+      </c>
+      <c r="P12">
+        <v>90</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>311</v>
       </c>
@@ -2623,8 +2893,15 @@
       <c r="M13" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13" s="12"/>
+      <c r="O13" t="s">
+        <v>89</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>312</v>
       </c>
@@ -2664,8 +2941,21 @@
       <c r="M14" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14" s="12"/>
+      <c r="O14" t="s">
+        <v>206</v>
+      </c>
+      <c r="P14">
+        <v>360</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>313</v>
       </c>
@@ -2705,8 +2995,15 @@
       <c r="M15" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15" s="12"/>
+      <c r="O15" t="s">
+        <v>205</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>314</v>
       </c>
@@ -2746,8 +3043,15 @@
       <c r="M16" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="12"/>
+      <c r="O16" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>315</v>
       </c>
@@ -2787,8 +3091,15 @@
       <c r="M17" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="12"/>
+      <c r="O17" t="s">
+        <v>205</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>316</v>
       </c>
@@ -2828,8 +3139,15 @@
       <c r="M18" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18" s="12"/>
+      <c r="O18" t="s">
+        <v>205</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>317</v>
       </c>
@@ -2869,8 +3187,15 @@
       <c r="M19" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19" s="12"/>
+      <c r="O19" t="s">
+        <v>89</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>318</v>
       </c>
@@ -2910,8 +3235,15 @@
       <c r="M20" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20" s="12"/>
+      <c r="O20" t="s">
+        <v>89</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>319</v>
       </c>
@@ -2951,24 +3283,48 @@
       <c r="M21" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="N21" s="12"/>
+      <c r="O21" t="s">
+        <v>89</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A3:K11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K11">
     <sortCondition ref="A3:A11"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="P2:R2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:K1 A2 C2:K2 L1:M1048576 A3:K1048576">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <conditionalFormatting sqref="A2 L1:N1048576 A1:K1 C2:K2 A3:K1048576 P1">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$A2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O21">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$A2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:R21">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2977,12 +3333,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3150,15 +3503,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B3BB0C-36B2-46D3-88DC-D85AAEEDA53C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4614B039-1CD1-4631-99C8-FAFC36432D48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3182,10 +3539,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4614B039-1CD1-4631-99C8-FAFC36432D48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B3BB0C-36B2-46D3-88DC-D85AAEEDA53C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
shader pixel snapping off
</commit_message>
<xml_diff>
--- a/Project_C/Assets/ExcelTable/CardTable.xlsx
+++ b/Project_C/Assets/ExcelTable/CardTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Main\TeamIdentity\Project_C\Assets\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D2DEA7-1105-4305-BD16-88337D6BCB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D37C477-88C9-4899-A6B6-A4A964771BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4350" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="216">
   <si>
     <t>i_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -859,6 +859,10 @@
   </si>
   <si>
     <t>범위 스프라이트 이미지 경로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -965,6 +969,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -979,12 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2239,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2289,25 +2293,25 @@
       <c r="I1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="6" t="s">
         <v>213</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2355,11 +2359,11 @@
       <c r="O2" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -2401,7 +2405,9 @@
       <c r="M3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N3" s="12"/>
+      <c r="N3" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O3" t="s">
         <v>205</v>
       </c>
@@ -2455,9 +2461,17 @@
       <c r="M4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N4" s="12"/>
+      <c r="N4" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O4" t="s">
         <v>89</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -2503,9 +2517,17 @@
       <c r="M5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N5" s="12"/>
+      <c r="N5" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O5" t="s">
         <v>89</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2551,9 +2573,17 @@
       <c r="M6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N6" s="12"/>
+      <c r="N6" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O6" t="s">
         <v>89</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2599,9 +2629,17 @@
       <c r="M7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N7" s="12"/>
+      <c r="N7" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O7" t="s">
         <v>89</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -2647,9 +2685,17 @@
       <c r="M8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N8" s="12"/>
+      <c r="N8" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O8" t="s">
         <v>89</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -2695,9 +2741,17 @@
       <c r="M9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N9" s="12"/>
+      <c r="N9" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O9" t="s">
         <v>89</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -2743,9 +2797,17 @@
       <c r="M10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N10" s="12"/>
+      <c r="N10" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O10" t="s">
         <v>89</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -2791,9 +2853,17 @@
       <c r="M11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N11" s="12"/>
+      <c r="N11" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O11" t="s">
         <v>89</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -2839,7 +2909,9 @@
       <c r="M12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N12" s="12"/>
+      <c r="N12" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O12" t="s">
         <v>205</v>
       </c>
@@ -2893,9 +2965,17 @@
       <c r="M13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N13" s="12"/>
+      <c r="N13" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O13" t="s">
         <v>89</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -2941,7 +3021,9 @@
       <c r="M14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N14" s="12"/>
+      <c r="N14" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O14" t="s">
         <v>206</v>
       </c>
@@ -2995,9 +3077,17 @@
       <c r="M15" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N15" s="12"/>
+      <c r="N15" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O15" t="s">
         <v>205</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -3043,9 +3133,17 @@
       <c r="M16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N16" s="12"/>
+      <c r="N16" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O16" t="s">
         <v>89</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -3091,9 +3189,17 @@
       <c r="M17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N17" s="12"/>
+      <c r="N17" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O17" t="s">
         <v>205</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -3139,9 +3245,17 @@
       <c r="M18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N18" s="12"/>
+      <c r="N18" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O18" t="s">
         <v>205</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -3187,9 +3301,17 @@
       <c r="M19" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O19" t="s">
         <v>89</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -3235,9 +3357,17 @@
       <c r="M20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N20" s="12"/>
+      <c r="N20" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O20" t="s">
         <v>89</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -3283,9 +3413,17 @@
       <c r="M21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N21" s="12"/>
+      <c r="N21" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="O21" t="s">
         <v>89</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -3302,7 +3440,7 @@
     <mergeCell ref="P2:R2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2 L1:N1048576 A1:K1 C2:K2 A3:K1048576 P1">
+  <conditionalFormatting sqref="A2 A1:K1 C2:K2 A3:K1048576 P1 L1:N1048576">
     <cfRule type="expression" dxfId="4" priority="7">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -3333,9 +3471,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3503,19 +3644,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4614B039-1CD1-4631-99C8-FAFC36432D48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B3BB0C-36B2-46D3-88DC-D85AAEEDA53C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3539,9 +3676,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B3BB0C-36B2-46D3-88DC-D85AAEEDA53C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4614B039-1CD1-4631-99C8-FAFC36432D48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cardrangeinterface 추가, range 이름 변경
</commit_message>
<xml_diff>
--- a/Project_C/Assets/ExcelTable/CardTable.xlsx
+++ b/Project_C/Assets/ExcelTable/CardTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Main\TeamIdentity\Project_C\Assets\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D37C477-88C9-4899-A6B6-A4A964771BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECDD541-6694-4388-9D49-9FCE25E4134B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4350" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="218">
   <si>
     <t>i_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -838,14 +838,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>범위 파라미터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_RangeParameter[3]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>파라미터 x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -863,6 +855,22 @@
   </si>
   <si>
     <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Range/powerattack_range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Range/groundpowerattack_range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Range/everybodyslime_range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Range/counter_range</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -901,7 +909,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -935,22 +943,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -978,59 +977,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <border>
         <left style="thin">
@@ -1807,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1821,7 +1772,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1835,7 +1786,7 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2018,7 +1969,7 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2230,7 +2181,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2241,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2260,12 +2211,11 @@
     <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.75" customWidth="1"/>
     <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,18 +2252,13 @@
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2354,18 +2299,13 @@
         <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>301</v>
       </c>
@@ -2406,22 +2346,13 @@
         <v>0</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O3" t="s">
         <v>205</v>
       </c>
-      <c r="P3">
-        <v>160</v>
-      </c>
-      <c r="Q3">
-        <v>1.8</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>302</v>
       </c>
@@ -2462,22 +2393,13 @@
         <v>0</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O4" t="s">
         <v>89</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>303</v>
       </c>
@@ -2518,22 +2440,13 @@
         <v>0</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O5" t="s">
         <v>89</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>304</v>
       </c>
@@ -2574,22 +2487,13 @@
         <v>0</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O6" t="s">
         <v>89</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>305</v>
       </c>
@@ -2630,22 +2534,13 @@
         <v>0</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O7" t="s">
         <v>89</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>306</v>
       </c>
@@ -2686,22 +2581,13 @@
         <v>0</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O8" t="s">
         <v>89</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>307</v>
       </c>
@@ -2742,22 +2628,13 @@
         <v>0</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O9" t="s">
         <v>89</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>308</v>
       </c>
@@ -2798,22 +2675,13 @@
         <v>0</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O10" t="s">
         <v>89</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>309</v>
       </c>
@@ -2854,22 +2722,13 @@
         <v>0</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O11" t="s">
         <v>89</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>310</v>
       </c>
@@ -2915,17 +2774,8 @@
       <c r="O12" t="s">
         <v>205</v>
       </c>
-      <c r="P12">
-        <v>90</v>
-      </c>
-      <c r="Q12">
-        <v>3</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>311</v>
       </c>
@@ -2966,22 +2816,13 @@
         <v>0</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O13" t="s">
         <v>89</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>312</v>
       </c>
@@ -3022,22 +2863,13 @@
         <v>0</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O14" t="s">
         <v>206</v>
       </c>
-      <c r="P14">
-        <v>360</v>
-      </c>
-      <c r="Q14">
-        <v>2</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>313</v>
       </c>
@@ -3078,22 +2910,13 @@
         <v>0</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O15" t="s">
         <v>205</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>314</v>
       </c>
@@ -3134,22 +2957,13 @@
         <v>0</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O16" t="s">
         <v>89</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>315</v>
       </c>
@@ -3190,22 +3004,13 @@
         <v>0</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="O17" t="s">
         <v>205</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>316</v>
       </c>
@@ -3246,22 +3051,13 @@
         <v>0</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O18" t="s">
         <v>205</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>317</v>
       </c>
@@ -3302,22 +3098,13 @@
         <v>0</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O19" t="s">
         <v>89</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>318</v>
       </c>
@@ -3358,22 +3145,13 @@
         <v>0</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O20" t="s">
         <v>89</v>
       </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>319</v>
       </c>
@@ -3414,55 +3192,34 @@
         <v>0</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O21" t="s">
         <v>89</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K11">
     <sortCondition ref="A3:A11"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="P2:R2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2 A1:K1 C2:K2 A3:K1048576 P1 L1:N1048576">
-    <cfRule type="expression" dxfId="4" priority="7">
+  <conditionalFormatting sqref="A2 A1:K1 C2:K2 A3:K1048576 L1:N1048576">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O21">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$A1&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$A2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:R21">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
anim angle code 수정
</commit_message>
<xml_diff>
--- a/Project_C/Assets/ExcelTable/CardTable.xlsx
+++ b/Project_C/Assets/ExcelTable/CardTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Main\TeamIdentity\Project_C\Assets\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65985E2-E2A4-4703-8DB7-28303DA7875C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F0552A-9FC8-41FC-BE26-39E961247FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2216,7 +2216,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2887,7 +2887,7 @@
         <v>217</v>
       </c>
       <c r="O14" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3249,9 +3249,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3419,19 +3422,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4614B039-1CD1-4631-99C8-FAFC36432D48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B3BB0C-36B2-46D3-88DC-D85AAEEDA53C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3455,9 +3454,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B3BB0C-36B2-46D3-88DC-D85AAEEDA53C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4614B039-1CD1-4631-99C8-FAFC36432D48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>